<commit_message>
Birds Product testcases updated by Team-A
</commit_message>
<xml_diff>
--- a/QKP-SJFJVD-A8/src/main/resources/ReffrenceDocument/TestData_A8.xlsx
+++ b/QKP-SJFJVD-A8/src/main/resources/ReffrenceDocument/TestData_A8.xlsx
@@ -1,37 +1,212 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/14b3b942826af451/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B53164C-5039-4495-85A7-30DF44F63B42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3980" firstSheet="1" activeTab="4" xr2:uid="{FB2D2CC8-83FE-4CFB-BADA-23D2708F0ABD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="3984"/>
   </bookViews>
   <sheets>
-    <sheet name="DogsProduct-TeamA" sheetId="1" r:id="rId1"/>
+    <sheet name="BirdsProduct-TeamA" sheetId="1" r:id="rId1"/>
     <sheet name="ReptilesProduct-TeamB" sheetId="2" r:id="rId2"/>
     <sheet name="CatsProduct-TeamC" sheetId="3" r:id="rId3"/>
     <sheet name="FishProduct-TeamD" sheetId="4" r:id="rId4"/>
     <sheet name="BirdsProduct-TeamE" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+  <si>
+    <t>Testcase ID</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PreCondition</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>Approved By</t>
+  </si>
+  <si>
+    <t>T001</t>
+  </si>
+  <si>
+    <t>Open Petstore Demo - 
+OctoPerf Application</t>
+  </si>
+  <si>
+    <t>Birds Module</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Welcome to JPetStore page must be displayed</t>
+  </si>
+  <si>
+    <t>Click on Enter the Store</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>JPetStore home 
+must be displayed</t>
+  </si>
+  <si>
+    <t>Click on Sign In</t>
+  </si>
+  <si>
+    <t>Sign In page must be displayed</t>
+  </si>
+  <si>
+    <t>Enter Username and 
+Password</t>
+  </si>
+  <si>
+    <t>Username: Tejakommi
+Password: Yathwik@123</t>
+  </si>
+  <si>
+    <t>Click on Login</t>
+  </si>
+  <si>
+    <t>Home page must  be displayed</t>
+  </si>
+  <si>
+    <t>Click on Birds</t>
+  </si>
+  <si>
+    <t>Birds page should display</t>
+  </si>
+  <si>
+    <t>Click on AV-CB-01</t>
+  </si>
+  <si>
+    <t>Amazon Parrot page should display</t>
+  </si>
+  <si>
+    <t>Click on Add to Cart</t>
+  </si>
+  <si>
+    <t>Shopping Cart page should dislay</t>
+  </si>
+  <si>
+    <t>Clear the text in the 
+Quantity field</t>
+  </si>
+  <si>
+    <t>Enter number in the Quantity 
+field</t>
+  </si>
+  <si>
+    <t>20 should entered in the Quantity field</t>
+  </si>
+  <si>
+    <t>Click on Update Cart</t>
+  </si>
+  <si>
+    <t>Total Cost should
+ get updated</t>
+  </si>
+  <si>
+    <t>Click on Proceed to 
+Checkout</t>
+  </si>
+  <si>
+    <t>Click on Continue</t>
+  </si>
+  <si>
+    <t>Order page should
+ get displayed</t>
+  </si>
+  <si>
+    <t>Click on Confirm</t>
+  </si>
+  <si>
+    <t>Click on Remove</t>
+  </si>
+  <si>
+    <t>"Order has been Submitted" message should get displayed</t>
+  </si>
+  <si>
+    <t>Click on Sign Out</t>
+  </si>
+  <si>
+    <t>Account should be created</t>
+  </si>
+  <si>
+    <t>Account should be created and Product should be present in the cart</t>
+  </si>
+  <si>
+    <t>Order should be 
+placed  Successfully</t>
+  </si>
+  <si>
+    <t>Cart should be Empty</t>
+  </si>
+  <si>
+    <t>Username and Password should entered in textfield</t>
+  </si>
+  <si>
+    <t>Payment Details page should get displayed</t>
+  </si>
+  <si>
+    <t>In Shopping Cart page "Your cart is empty" Message should get displayed</t>
+  </si>
+  <si>
+    <t>url: https://petstore.octoperf.com</t>
+  </si>
+  <si>
+    <t>Lavanya</t>
+  </si>
+  <si>
+    <t>Tejaswini</t>
+  </si>
+  <si>
+    <t>T002</t>
+  </si>
+  <si>
+    <t>text should be cleared</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,16 +214,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -56,14 +253,153 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -71,9 +407,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -368,79 +701,783 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2496394F-3B5A-4FBF-86CC-8781839AB230}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="23"/>
+    </row>
+    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="28"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="28"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="28"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="28"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="28"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="28"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="28"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="10">
+        <v>20</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="28"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="31"/>
+      <c r="H16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="19"/>
+    </row>
+    <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" s="6"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="30"/>
+      <c r="H19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="26"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="30"/>
+      <c r="H22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="30"/>
+      <c r="H24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="10">
+        <v>20</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="31"/>
+      <c r="H28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="G2:G16"/>
+    <mergeCell ref="G18:G28"/>
+    <mergeCell ref="K2:K16"/>
+    <mergeCell ref="K18:K28"/>
+    <mergeCell ref="L2:L16"/>
+    <mergeCell ref="L18:L28"/>
+    <mergeCell ref="A18:A28"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="B2:B16"/>
+    <mergeCell ref="B18:B28"/>
+    <mergeCell ref="D2:D16"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="D18:D28"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="url:https://petstore.octoperf.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432FB32D-1A13-4296-AD2F-FB274D83480F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6149C2-7D87-43C5-9685-1A1E1D4CBE34}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4165F6-93AC-4B8C-A891-66BF675FFFE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8573B9-1B36-46C4-A1A3-5D0703F3712F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F529D7-D38C-4995-9379-680868B087C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>